<commit_message>
Add virtually pdf files
</commit_message>
<xml_diff>
--- a/data/RawData/ObsData/2001-2009/01-01-2005.xlsx
+++ b/data/RawData/ObsData/2001-2009/01-01-2005.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aponchon\Nextcloud\Aurore Ponchon\Projects\Golden Lion Tamarins Brazil\Analysis\GoldenLionTamarins\data\RawData\ObsData\2001-2009\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4973DE3-FC68-4BCA-9EF6-9D429988A476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE55FE6-352E-4B41-B7A4-6AB272ADF028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2852" uniqueCount="1040">
   <si>
     <t>Micos Reintro Jan-2005</t>
   </si>
@@ -5420,8 +5420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R392"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N110" sqref="N110"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="L154" sqref="L154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10694,8 +10694,8 @@
         <v>497</v>
       </c>
       <c r="K153" s="14"/>
-      <c r="L153" s="14" t="s">
-        <v>535</v>
+      <c r="L153" t="s">
+        <v>19</v>
       </c>
       <c r="M153" s="14" t="s">
         <v>19</v>
@@ -10730,7 +10730,7 @@
       </c>
       <c r="K154" s="14"/>
       <c r="L154" s="14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="M154" s="14" t="s">
         <v>11</v>
@@ -10761,7 +10761,7 @@
       </c>
       <c r="K155" s="14"/>
       <c r="L155" s="14" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="M155" s="14" t="s">
         <v>11</v>
@@ -10791,8 +10791,8 @@
         <v>537</v>
       </c>
       <c r="K156" s="17"/>
-      <c r="L156" s="17" t="s">
-        <v>538</v>
+      <c r="L156" s="14" t="s">
+        <v>537</v>
       </c>
       <c r="M156" s="17" t="s">
         <v>19</v>
@@ -10822,7 +10822,9 @@
         <v>538</v>
       </c>
       <c r="K157" s="17"/>
-      <c r="L157" s="17"/>
+      <c r="L157" s="17" t="s">
+        <v>538</v>
+      </c>
       <c r="M157" s="17" t="s">
         <v>19</v>
       </c>

</xml_diff>